<commit_message>
nov 18. updated analysis and new data
</commit_message>
<xml_diff>
--- a/external data/Chatfield-Reed 2022/jkac194_table_s6.xlsx
+++ b/external data/Chatfield-Reed 2022/jkac194_table_s6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mostl\OneDrive\Desktop\SGAPaper_5_20_22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcbtkov_ucl_ac_uk/Documents/MSci Bahler lab/S.-Pombe-biofilm/external data/Chatfield-Reed 2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0F3E4A-E1DF-4F37-A666-18A4E14CA970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="38700" windowHeight="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -666,14 +666,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -687,7 +689,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -698,7 +700,7 @@
         <v>-1.1890000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -709,7 +711,7 @@
         <v>-0.65700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -720,7 +722,7 @@
         <v>-0.59499999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -731,7 +733,7 @@
         <v>-0.56799999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -742,7 +744,7 @@
         <v>-0.55900000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -753,7 +755,7 @@
         <v>-0.55300000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -764,7 +766,7 @@
         <v>-0.52900000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -778,7 +780,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -789,7 +791,7 @@
         <v>-0.504</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -800,7 +802,7 @@
         <v>-0.79500000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -811,7 +813,7 @@
         <v>-0.68899999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -822,7 +824,7 @@
         <v>-0.64300000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -833,7 +835,7 @@
         <v>-0.60799999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -844,7 +846,7 @@
         <v>-0.60299999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -855,7 +857,7 @@
         <v>-0.59899999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -866,7 +868,7 @@
         <v>-0.58899999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -877,7 +879,7 @@
         <v>-0.56200000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -888,7 +890,7 @@
         <v>-0.55900000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -899,7 +901,7 @@
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -910,7 +912,7 @@
         <v>-0.52800000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -921,7 +923,7 @@
         <v>-0.52500000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -932,7 +934,7 @@
         <v>-0.51800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -943,7 +945,7 @@
         <v>-0.50600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -954,7 +956,7 @@
         <v>-0.89800000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -965,7 +967,7 @@
         <v>-0.73</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -976,7 +978,7 @@
         <v>-0.70699999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -987,7 +989,7 @@
         <v>-0.61799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>-0.59199999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>-0.59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>-0.51900000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>-0.51300000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -1042,7 +1044,7 @@
         <v>-0.72699999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -1056,7 +1058,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -1067,7 +1069,7 @@
         <v>-0.56000000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>103</v>
       </c>
@@ -1078,7 +1080,7 @@
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -1089,7 +1091,7 @@
         <v>-0.54400000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>103</v>
       </c>
@@ -1100,7 +1102,7 @@
         <v>-0.51200000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -1111,7 +1113,7 @@
         <v>-0.51</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -1122,7 +1124,7 @@
         <v>-0.51</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1136,7 +1138,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1150,7 +1152,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1163,7 @@
         <v>-0.75600000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1175,7 +1177,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -1189,7 +1191,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1203,7 +1205,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -1245,7 +1247,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1261,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1289,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -1298,7 +1300,7 @@
         <v>-0.77800000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1312,7 +1314,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>-0.76500000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1337,7 +1339,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -1348,7 +1350,7 @@
         <v>-0.73499999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>-0.71199999999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -1387,7 +1389,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -1398,7 +1400,7 @@
         <v>-0.64</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -1409,7 +1411,7 @@
         <v>-0.60399999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -1420,7 +1422,7 @@
         <v>-0.59799999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>-0.55900000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1444,7 @@
         <v>-0.55600000000000005</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1455,7 @@
         <v>-0.54400000000000004</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -1464,7 +1466,7 @@
         <v>-0.54200000000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -1475,7 +1477,7 @@
         <v>-0.53100000000000003</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -1486,7 +1488,7 @@
         <v>-0.51100000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1497,7 +1499,7 @@
         <v>-0.92800000000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>-0.70699999999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>-0.66900000000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1530,7 +1532,7 @@
         <v>-0.60899999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -1541,7 +1543,7 @@
         <v>-0.60699999999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -1555,7 +1557,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -1566,7 +1568,7 @@
         <v>-0.59299999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -1577,7 +1579,7 @@
         <v>-0.59</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1590,7 @@
         <v>-0.56200000000000006</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1599,7 +1601,7 @@
         <v>-0.54800000000000004</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -1610,7 +1612,7 @@
         <v>-0.52500000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -1621,7 +1623,7 @@
         <v>-0.503</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -1632,7 +1634,7 @@
         <v>-0.88400000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -1643,7 +1645,7 @@
         <v>-0.63300000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +1656,7 @@
         <v>-0.61699999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -1665,7 +1667,7 @@
         <v>-0.54800000000000004</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -1676,7 +1678,7 @@
         <v>-0.54600000000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>-0.53900000000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -1698,7 +1700,7 @@
         <v>-0.53</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>-0.52900000000000003</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -1720,7 +1722,7 @@
         <v>-0.52800000000000002</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -1731,7 +1733,7 @@
         <v>-0.52200000000000002</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +1744,7 @@
         <v>-0.51500000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -1753,7 +1755,7 @@
         <v>-0.51300000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -1764,7 +1766,7 @@
         <v>-1.0629999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -1775,7 +1777,7 @@
         <v>-1.012</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -1786,7 +1788,7 @@
         <v>-0.88300000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -1797,7 +1799,7 @@
         <v>-0.84099999999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -1808,7 +1810,7 @@
         <v>-0.81399999999999995</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -1819,7 +1821,7 @@
         <v>-0.73799999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1832,7 @@
         <v>-0.65300000000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>-0.61799999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1852,7 +1854,7 @@
         <v>-0.61599999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -1863,7 +1865,7 @@
         <v>-0.58599999999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>-0.57999999999999996</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -1885,7 +1887,7 @@
         <v>-0.52800000000000002</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>7</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>-0.52500000000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>-0.51100000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>7</v>
       </c>
@@ -1918,7 +1920,7 @@
         <v>-0.50600000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -1929,7 +1931,7 @@
         <v>-0.502</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>-1.32</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -1951,7 +1953,7 @@
         <v>-0.82299999999999995</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -1976,7 +1978,7 @@
         <v>-0.70299999999999996</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -1987,7 +1989,7 @@
         <v>-0.68200000000000005</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>-0.65500000000000003</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -2009,7 +2011,7 @@
         <v>-0.64</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>-0.623</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>-0.61199999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>-0.58899999999999997</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -2067,7 +2069,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -2078,7 +2080,7 @@
         <v>-0.54700000000000004</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -2089,7 +2091,7 @@
         <v>-0.53300000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -2100,7 +2102,7 @@
         <v>-0.53</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -2111,7 +2113,7 @@
         <v>-0.51900000000000002</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -2122,7 +2124,7 @@
         <v>-0.51400000000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>8</v>
       </c>
@@ -2133,7 +2135,7 @@
         <v>-0.50900000000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>-0.504</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -2155,7 +2157,7 @@
         <v>-0.97499999999999998</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>9</v>
       </c>
@@ -2166,7 +2168,7 @@
         <v>-0.91300000000000003</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -2177,7 +2179,7 @@
         <v>-0.74099999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -2188,7 +2190,7 @@
         <v>-0.71199999999999997</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>9</v>
       </c>
@@ -2199,7 +2201,7 @@
         <v>-0.67300000000000004</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>9</v>
       </c>
@@ -2210,7 +2212,7 @@
         <v>-0.66300000000000003</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -2221,7 +2223,7 @@
         <v>-0.66100000000000003</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>-0.64600000000000002</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -2243,7 +2245,7 @@
         <v>-0.60799999999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>9</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v>-0.60099999999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>-0.58299999999999996</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -2276,7 +2278,7 @@
         <v>-0.57499999999999996</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -2287,7 +2289,7 @@
         <v>-0.57199999999999995</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -2298,7 +2300,7 @@
         <v>-0.56000000000000005</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -2309,7 +2311,7 @@
         <v>-0.52600000000000002</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -2320,7 +2322,7 @@
         <v>-0.51800000000000002</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>10</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>-0.996</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -2345,7 +2347,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>10</v>
       </c>
@@ -2359,7 +2361,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>10</v>
       </c>
@@ -2387,7 +2389,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>10</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>10</v>
       </c>
@@ -2415,7 +2417,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>10</v>
       </c>
@@ -2429,7 +2431,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -2443,7 +2445,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>10</v>
       </c>
@@ -2454,7 +2456,7 @@
         <v>-0.54800000000000004</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -2468,7 +2470,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -2479,7 +2481,7 @@
         <v>-0.54400000000000004</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -2490,7 +2492,7 @@
         <v>-0.53</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -2501,7 +2503,7 @@
         <v>-0.51400000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -2512,7 +2514,7 @@
         <v>-0.51300000000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -2523,7 +2525,7 @@
         <v>-0.504</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>11</v>
       </c>
@@ -2534,7 +2536,7 @@
         <v>-1.3440000000000001</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -2548,7 +2550,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -2559,7 +2561,7 @@
         <v>-0.73499999999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>11</v>
       </c>
@@ -2571,7 +2573,7 @@
       </c>
       <c r="D164" s="1"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>11</v>
       </c>
@@ -2583,7 +2585,7 @@
       </c>
       <c r="D165" s="1"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>11</v>
       </c>
@@ -2595,7 +2597,7 @@
       </c>
       <c r="D166" s="1"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>11</v>
       </c>
@@ -2607,7 +2609,7 @@
       </c>
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>11</v>
       </c>
@@ -2619,7 +2621,7 @@
       </c>
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>11</v>
       </c>
@@ -2633,7 +2635,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>11</v>
       </c>
@@ -2647,7 +2649,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>11</v>
       </c>
@@ -2661,7 +2663,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>11</v>
       </c>
@@ -2673,7 +2675,7 @@
       </c>
       <c r="D172" s="1"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>11</v>
       </c>
@@ -2685,7 +2687,7 @@
       </c>
       <c r="D173" s="1"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>11</v>
       </c>
@@ -2699,7 +2701,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -2710,7 +2712,7 @@
         <v>-0.51</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -2721,7 +2723,7 @@
         <v>-0.51</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -2732,7 +2734,7 @@
         <v>-0.503</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>12</v>
       </c>
@@ -2743,7 +2745,7 @@
         <v>-1.2030000000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>12</v>
       </c>
@@ -2754,7 +2756,7 @@
         <v>-1.028</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>12</v>
       </c>
@@ -2768,7 +2770,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>12</v>
       </c>
@@ -2782,7 +2784,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>12</v>
       </c>
@@ -2796,7 +2798,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>12</v>
       </c>
@@ -2810,7 +2812,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>12</v>
       </c>
@@ -2824,7 +2826,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>12</v>
       </c>
@@ -2838,7 +2840,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>12</v>
       </c>
@@ -2852,7 +2854,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>12</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>12</v>
       </c>
@@ -2880,7 +2882,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>12</v>
       </c>
@@ -2894,7 +2896,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>12</v>
       </c>
@@ -2908,7 +2910,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>12</v>
       </c>
@@ -2922,7 +2924,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>12</v>
       </c>
@@ -2936,7 +2938,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>12</v>
       </c>
@@ -2950,7 +2952,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>12</v>
       </c>
@@ -2964,7 +2966,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>12</v>
       </c>
@@ -2978,7 +2980,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>12</v>
       </c>

</xml_diff>